<commit_message>
combined marraige and regular data
</commit_message>
<xml_diff>
--- a/full_data/marriage_data.xlsx
+++ b/full_data/marriage_data.xlsx
@@ -8,14 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gracegao/Desktop/BassConnections/full_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915A54E4-1E9C-F145-A9E1-83266FB51FB4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05582CCE-1A67-ED4D-B558-1E21DE48209C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4540" yWindow="8400" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33180" yWindow="2420" windowWidth="16100" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -471,7 +482,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -490,7 +503,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>

</xml_diff>